<commit_message>
minor changes with clear_db
</commit_message>
<xml_diff>
--- a/discord_bot/export/Butcher#1432.xlsx
+++ b/discord_bot/export/Butcher#1432.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="136">
   <si>
     <t>message_id</t>
   </si>
@@ -394,6 +394,42 @@
   </si>
   <si>
     <t>2021-09-12 15:52:44.926000</t>
+  </si>
+  <si>
+    <t>2021-09-12 16:09:07.919000</t>
+  </si>
+  <si>
+    <t>/get_all</t>
+  </si>
+  <si>
+    <t>2021-09-13 08:40:23.295000</t>
+  </si>
+  <si>
+    <t>2021-09-13 08:41:13.335000</t>
+  </si>
+  <si>
+    <t>2021-09-13 08:42:32.656000</t>
+  </si>
+  <si>
+    <t>2021-09-13 08:43:03.417000</t>
+  </si>
+  <si>
+    <t>2021-09-13 08:43:30.786000</t>
+  </si>
+  <si>
+    <t>2021-09-13 08:44:01.394000</t>
+  </si>
+  <si>
+    <t>2021-09-13 08:44:34.845000</t>
+  </si>
+  <si>
+    <t>2021-09-13 08:44:52.933000</t>
+  </si>
+  <si>
+    <t>2021-09-13 08:45:26.160000</t>
+  </si>
+  <si>
+    <t>2021-09-14 07:55:14.929000</t>
   </si>
 </sst>
 </file>
@@ -754,7 +790,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2124,6 +2160,193 @@
         <v>13</v>
       </c>
     </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="2">
+        <v>94</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="2">
+        <v>95</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="2">
+        <v>96</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" s="2">
+        <v>97</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" s="2">
+        <v>98</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="2">
+        <v>99</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="2">
+        <v>100</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="2">
+        <v>101</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="2">
+        <v>102</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="2">
+        <v>103</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="2">
+        <v>104</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>